<commit_message>
hotfix: some fixes for importing
</commit_message>
<xml_diff>
--- a/Modules/ACC/database/seeders/Samad Accounts List STD fixed.xlsx
+++ b/Modules/ACC/database/seeders/Samad Accounts List STD fixed.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="97">
   <si>
     <t xml:space="preserve">cat_id</t>
   </si>
@@ -66,6 +66,9 @@
     <t xml:space="preserve">moein_name</t>
   </si>
   <si>
+    <t xml:space="preserve">new_chain_moein</t>
+  </si>
+  <si>
     <t xml:space="preserve">دارائیهای جاری</t>
   </si>
   <si>
@@ -105,10 +108,10 @@
     <t xml:space="preserve">سایر حسابهای دریافتنی</t>
   </si>
   <si>
-    <t xml:space="preserve">خسارات قابل دریافت ازبیمه</t>
-  </si>
-  <si>
-    <t xml:space="preserve">پیش پرداختها</t>
+    <t xml:space="preserve">خسارات قابل دریافت از بیمه</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ودایع و پیش پرداخت ها</t>
   </si>
   <si>
     <t xml:space="preserve">پیش پرداخت هزینه‌ های جاری</t>
@@ -422,13 +425,138 @@
   <si>
     <t xml:space="preserve">سپرده مناقصه و مزایده</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">5% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Vazirmatn"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">حسن انجام کار پیمانکاران</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">علی الحساب</t>
+  </si>
+  <si>
+    <t xml:space="preserve">علی الحساب پرداختنی به پیمانکاران</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Vazirmatn"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">کسورات قانونی </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Vazirmatn"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">حق بیمه</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">حسابهای انتظامی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">حساب انتظامی سرمایه گذاریها</t>
+  </si>
+  <si>
+    <t xml:space="preserve">حساب انتظامی سرمایه‌گذاری در شرکت های تعاونی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">طرف حساب انتظامی سرمایه گذاریها</t>
+  </si>
+  <si>
+    <t xml:space="preserve">طرف حساب انتظامی سرمایه‌گذاری در شرکت های تعاونی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">موجودی مصالح و لوازم</t>
+  </si>
+  <si>
+    <t xml:space="preserve">سیمان</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شن و ماسه</t>
+  </si>
+  <si>
+    <t xml:space="preserve">سنگ لاشه</t>
+  </si>
+  <si>
+    <t xml:space="preserve">جدول</t>
+  </si>
+  <si>
+    <t xml:space="preserve">پلاک بتنی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">آجر فشاری</t>
+  </si>
+  <si>
+    <t xml:space="preserve">حساب انتظامی دارائیها</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">حساب انتظامی اداری و نرم افزار</t>
+  </si>
+  <si>
+    <t xml:space="preserve">طرف حساب انتظامی دارائیها</t>
+  </si>
+  <si>
+    <t xml:space="preserve">طرف حساب انتظامی اداری و نرم‌افزار</t>
+  </si>
+  <si>
+    <t xml:space="preserve">سنگ مالون</t>
+  </si>
+  <si>
+    <t xml:space="preserve">حق السهم حقوق و دستمزد پرداختنی سایر کارکنان</t>
+  </si>
+  <si>
+    <t xml:space="preserve">وجوه مسدود شده</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -508,7 +636,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -517,8 +645,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -543,8 +683,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="new" displayName="new" ref="A1:H46" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:H46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="new" displayName="new" ref="A1:H68" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:H68"/>
   <tableColumns count="8">
     <tableColumn id="1" name="cat_id"/>
     <tableColumn id="2" name="cat_name"/>
@@ -735,10 +875,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B73" activeCellId="0" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -749,7 +889,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="28.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="38.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="38.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="53.18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -762,7 +903,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -777,1265 +918,1448 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="n">
         <v>110</v>
       </c>
-      <c r="D2" s="2" t="str">
+      <c r="D2" s="4" t="str">
         <f aca="false">RIGHT(C2,2)</f>
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>110001</v>
+      </c>
+      <c r="G2" s="3" t="str">
+        <f aca="false">RIGHT(F2,2)</f>
+        <v>01</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>11001</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="n">
-        <v>110001</v>
-      </c>
-      <c r="G2" s="2" t="str">
-        <f aca="false">RIGHT(F2,3)</f>
-        <v>001</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="3" t="n">
         <v>110</v>
       </c>
-      <c r="D3" s="2" t="str">
+      <c r="D3" s="4" t="str">
         <f aca="false">RIGHT(C3,2)</f>
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>110003</v>
+      </c>
+      <c r="G3" s="3" t="str">
+        <f aca="false">RIGHT(F3,2)</f>
+        <v>03</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>11003</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="2" t="n">
-        <v>110003</v>
-      </c>
-      <c r="G3" s="2" t="str">
-        <f aca="false">RIGHT(F3,3)</f>
-        <v>003</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="3" t="n">
         <v>110</v>
       </c>
-      <c r="D4" s="2" t="str">
+      <c r="D4" s="4" t="str">
         <f aca="false">RIGHT(C4,2)</f>
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>110005</v>
+      </c>
+      <c r="G4" s="3" t="str">
+        <f aca="false">RIGHT(F4,2)</f>
+        <v>05</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>11005</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="2" t="n">
-        <v>110005</v>
-      </c>
-      <c r="G4" s="2" t="str">
-        <f aca="false">RIGHT(F4,3)</f>
-        <v>005</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="3" t="n">
         <v>112</v>
       </c>
-      <c r="D5" s="2" t="str">
+      <c r="D5" s="4" t="str">
         <f aca="false">RIGHT(C5,2)</f>
         <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="n">
         <v>112201</v>
       </c>
-      <c r="G5" s="2" t="str">
-        <f aca="false">RIGHT(F5,3)</f>
-        <v>201</v>
+      <c r="G5" s="3" t="str">
+        <f aca="false">RIGHT(F5,2)</f>
+        <v>01</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>11201</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="n">
         <v>112</v>
       </c>
-      <c r="D6" s="2" t="str">
+      <c r="D6" s="4" t="str">
         <f aca="false">RIGHT(C6,2)</f>
         <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3" t="n">
         <v>112202</v>
       </c>
-      <c r="G6" s="2" t="str">
-        <f aca="false">RIGHT(F6,3)</f>
-        <v>202</v>
+      <c r="G6" s="3" t="str">
+        <f aca="false">RIGHT(F6,2)</f>
+        <v>02</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>11202</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
+      <c r="A7" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="n">
         <v>112</v>
       </c>
-      <c r="D7" s="2" t="str">
+      <c r="D7" s="4" t="str">
         <f aca="false">RIGHT(C7,2)</f>
         <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="F7" s="3" t="n">
         <v>112203</v>
       </c>
-      <c r="G7" s="2" t="str">
-        <f aca="false">RIGHT(F7,3)</f>
-        <v>203</v>
+      <c r="G7" s="3" t="str">
+        <f aca="false">RIGHT(F7,2)</f>
+        <v>03</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>11203</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
+      <c r="A8" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="n">
         <v>112</v>
       </c>
-      <c r="D8" s="2" t="str">
+      <c r="D8" s="4" t="str">
         <f aca="false">RIGHT(C8,2)</f>
         <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="F8" s="3" t="n">
         <v>112204</v>
       </c>
-      <c r="G8" s="2" t="str">
-        <f aca="false">RIGHT(F8,3)</f>
-        <v>204</v>
+      <c r="G8" s="3" t="str">
+        <f aca="false">RIGHT(F8,2)</f>
+        <v>04</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>11204</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="n">
+      <c r="A9" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="n">
         <v>112</v>
       </c>
-      <c r="D9" s="2" t="str">
+      <c r="D9" s="4" t="str">
         <f aca="false">RIGHT(C9,2)</f>
         <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="F9" s="3" t="n">
         <v>112205</v>
       </c>
-      <c r="G9" s="2" t="str">
-        <f aca="false">RIGHT(F9,3)</f>
-        <v>205</v>
+      <c r="G9" s="3" t="str">
+        <f aca="false">RIGHT(F9,2)</f>
+        <v>05</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>11205</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="n">
+      <c r="A10" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="n">
         <v>113</v>
       </c>
-      <c r="D10" s="2" t="str">
+      <c r="D10" s="4" t="str">
         <f aca="false">RIGHT(C10,2)</f>
         <v>13</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="F10" s="3" t="n">
         <v>113304</v>
       </c>
-      <c r="G10" s="2" t="str">
-        <f aca="false">RIGHT(F10,3)</f>
-        <v>304</v>
+      <c r="G10" s="3" t="str">
+        <f aca="false">RIGHT(F10,2)</f>
+        <v>04</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>11304</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="n">
+      <c r="A11" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="n">
         <v>113</v>
       </c>
-      <c r="D11" s="2" t="str">
+      <c r="D11" s="4" t="str">
         <f aca="false">RIGHT(C11,2)</f>
         <v>13</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="F11" s="3" t="n">
         <v>113307</v>
       </c>
-      <c r="G11" s="2" t="str">
-        <f aca="false">RIGHT(F11,3)</f>
-        <v>307</v>
+      <c r="G11" s="3" t="str">
+        <f aca="false">RIGHT(F11,2)</f>
+        <v>07</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>11307</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="n">
+      <c r="A12" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3" t="n">
         <v>118</v>
       </c>
-      <c r="D12" s="2" t="str">
+      <c r="D12" s="4" t="str">
         <f aca="false">RIGHT(C12,2)</f>
         <v>18</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="F12" s="3" t="n">
         <v>118803</v>
       </c>
-      <c r="G12" s="2" t="str">
-        <f aca="false">RIGHT(F12,3)</f>
-        <v>803</v>
+      <c r="G12" s="3" t="str">
+        <f aca="false">RIGHT(F12,2)</f>
+        <v>03</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>11803</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="n">
+      <c r="A13" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="n">
         <v>118</v>
       </c>
-      <c r="D13" s="2" t="str">
+      <c r="D13" s="4" t="str">
         <f aca="false">RIGHT(C13,2)</f>
         <v>18</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="F13" s="3" t="n">
         <v>118808</v>
       </c>
-      <c r="G13" s="2" t="str">
-        <f aca="false">RIGHT(F13,3)</f>
-        <v>808</v>
+      <c r="G13" s="3" t="str">
+        <f aca="false">RIGHT(F13,2)</f>
+        <v>08</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>11808</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="n">
+      <c r="A14" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C14" s="3" t="n">
         <v>118</v>
       </c>
-      <c r="D14" s="2" t="str">
+      <c r="D14" s="4" t="str">
         <f aca="false">RIGHT(C14,2)</f>
         <v>18</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="F14" s="3" t="n">
         <v>118809</v>
       </c>
-      <c r="G14" s="2" t="str">
-        <f aca="false">RIGHT(F14,3)</f>
-        <v>809</v>
+      <c r="G14" s="3" t="str">
+        <f aca="false">RIGHT(F14,2)</f>
+        <v>09</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>11809</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="n">
+      <c r="A15" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C15" s="3" t="n">
         <v>310</v>
       </c>
-      <c r="D15" s="2" t="str">
+      <c r="D15" s="4" t="str">
         <f aca="false">RIGHT(C15,2)</f>
         <v>10</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="F15" s="3" t="n">
         <v>310001</v>
       </c>
-      <c r="G15" s="2" t="str">
-        <f aca="false">RIGHT(F15,3)</f>
-        <v>001</v>
+      <c r="G15" s="3" t="str">
+        <f aca="false">RIGHT(F15,2)</f>
+        <v>01</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="I15" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31001</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="n">
+      <c r="A16" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C16" s="3" t="n">
         <v>310</v>
       </c>
-      <c r="D16" s="2" t="str">
+      <c r="D16" s="4" t="str">
         <f aca="false">RIGHT(C16,2)</f>
         <v>10</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="F16" s="3" t="n">
         <v>310002</v>
       </c>
-      <c r="G16" s="2" t="str">
-        <f aca="false">RIGHT(F16,3)</f>
-        <v>002</v>
+      <c r="G16" s="3" t="str">
+        <f aca="false">RIGHT(F16,2)</f>
+        <v>02</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="I16" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31002</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="n">
+      <c r="A17" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C17" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D17" s="2" t="str">
+      <c r="D17" s="4" t="str">
         <f aca="false">RIGHT(C17,2)</f>
         <v>11</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="F17" s="3" t="n">
         <v>311101</v>
       </c>
-      <c r="G17" s="2" t="str">
-        <f aca="false">RIGHT(F17,3)</f>
-        <v>101</v>
+      <c r="G17" s="3" t="str">
+        <f aca="false">RIGHT(F17,2)</f>
+        <v>01</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="I17" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31101</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="n">
+      <c r="A18" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C18" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D18" s="2" t="str">
+      <c r="D18" s="4" t="str">
         <f aca="false">RIGHT(C18,2)</f>
         <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="F18" s="3" t="n">
         <v>311102</v>
       </c>
-      <c r="G18" s="2" t="str">
-        <f aca="false">RIGHT(F18,3)</f>
-        <v>102</v>
+      <c r="G18" s="3" t="str">
+        <f aca="false">RIGHT(F18,2)</f>
+        <v>02</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="I18" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31102</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="n">
+      <c r="A19" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D19" s="2" t="str">
+      <c r="D19" s="4" t="str">
         <f aca="false">RIGHT(C19,2)</f>
         <v>11</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="F19" s="3" t="n">
         <v>311103</v>
       </c>
-      <c r="G19" s="2" t="str">
-        <f aca="false">RIGHT(F19,3)</f>
-        <v>103</v>
+      <c r="G19" s="3" t="str">
+        <f aca="false">RIGHT(F19,2)</f>
+        <v>03</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="I19" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31103</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="n">
+      <c r="A20" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C20" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D20" s="2" t="str">
+      <c r="D20" s="4" t="str">
         <f aca="false">RIGHT(C20,2)</f>
         <v>11</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F20" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="F20" s="3" t="n">
         <v>311105</v>
       </c>
-      <c r="G20" s="2" t="str">
-        <f aca="false">RIGHT(F20,3)</f>
-        <v>105</v>
+      <c r="G20" s="3" t="str">
+        <f aca="false">RIGHT(F20,2)</f>
+        <v>05</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="I20" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31105</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="n">
+      <c r="A21" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C21" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D21" s="2" t="str">
+      <c r="D21" s="4" t="str">
         <f aca="false">RIGHT(C21,2)</f>
         <v>11</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="F21" s="3" t="n">
         <v>311106</v>
       </c>
-      <c r="G21" s="2" t="str">
-        <f aca="false">RIGHT(F21,3)</f>
-        <v>106</v>
+      <c r="G21" s="3" t="str">
+        <f aca="false">RIGHT(F21,2)</f>
+        <v>06</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="I21" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31106</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="n">
+      <c r="A22" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C22" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D22" s="2" t="str">
+      <c r="D22" s="4" t="str">
         <f aca="false">RIGHT(C22,2)</f>
         <v>11</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="F22" s="3" t="n">
         <v>311107</v>
       </c>
-      <c r="G22" s="2" t="str">
-        <f aca="false">RIGHT(F22,3)</f>
-        <v>107</v>
+      <c r="G22" s="3" t="str">
+        <f aca="false">RIGHT(F22,2)</f>
+        <v>07</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="I22" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31107</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="n">
+      <c r="A23" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C23" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D23" s="2" t="str">
+      <c r="D23" s="4" t="str">
         <f aca="false">RIGHT(C23,2)</f>
         <v>11</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F23" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="F23" s="3" t="n">
         <v>311108</v>
       </c>
-      <c r="G23" s="2" t="str">
-        <f aca="false">RIGHT(F23,3)</f>
-        <v>108</v>
+      <c r="G23" s="3" t="str">
+        <f aca="false">RIGHT(F23,2)</f>
+        <v>08</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="I23" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31108</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="n">
+      <c r="A24" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C24" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D24" s="2" t="str">
+      <c r="D24" s="4" t="str">
         <f aca="false">RIGHT(C24,2)</f>
         <v>11</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="F24" s="3" t="n">
         <v>311109</v>
       </c>
-      <c r="G24" s="2" t="str">
-        <f aca="false">RIGHT(F24,3)</f>
-        <v>109</v>
+      <c r="G24" s="3" t="str">
+        <f aca="false">RIGHT(F24,2)</f>
+        <v>09</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="I24" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31109</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="n">
+      <c r="A25" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C25" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D25" s="2" t="str">
+      <c r="D25" s="4" t="str">
         <f aca="false">RIGHT(C25,2)</f>
         <v>11</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F25" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="F25" s="3" t="n">
         <v>311110</v>
       </c>
-      <c r="G25" s="2" t="str">
-        <f aca="false">RIGHT(F25,3)</f>
-        <v>110</v>
+      <c r="G25" s="3" t="str">
+        <f aca="false">RIGHT(F25,2)</f>
+        <v>10</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="I25" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31110</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="n">
+      <c r="A26" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C26" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D26" s="2" t="str">
+      <c r="D26" s="4" t="str">
         <f aca="false">RIGHT(C26,2)</f>
         <v>11</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F26" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="F26" s="3" t="n">
         <v>311112</v>
       </c>
-      <c r="G26" s="2" t="str">
-        <f aca="false">RIGHT(F26,3)</f>
-        <v>112</v>
+      <c r="G26" s="3" t="str">
+        <f aca="false">RIGHT(F26,2)</f>
+        <v>12</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="I26" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31112</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="n">
+      <c r="A27" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C27" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D27" s="2" t="str">
+      <c r="D27" s="4" t="str">
         <f aca="false">RIGHT(C27,2)</f>
         <v>11</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F27" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="F27" s="3" t="n">
         <v>311115</v>
       </c>
-      <c r="G27" s="2" t="str">
-        <f aca="false">RIGHT(F27,3)</f>
-        <v>115</v>
+      <c r="G27" s="3" t="str">
+        <f aca="false">RIGHT(F27,2)</f>
+        <v>15</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="I27" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31115</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="n">
+      <c r="A28" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C28" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D28" s="2" t="str">
+      <c r="D28" s="4" t="str">
         <f aca="false">RIGHT(C28,2)</f>
         <v>11</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F28" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="F28" s="3" t="n">
         <v>311120</v>
       </c>
-      <c r="G28" s="2" t="str">
-        <f aca="false">RIGHT(F28,3)</f>
-        <v>120</v>
+      <c r="G28" s="3" t="str">
+        <f aca="false">RIGHT(F28,2)</f>
+        <v>20</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="I28" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31120</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="n">
+      <c r="A29" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C29" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D29" s="2" t="str">
+      <c r="D29" s="4" t="str">
         <f aca="false">RIGHT(C29,2)</f>
         <v>11</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F29" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="F29" s="3" t="n">
         <v>311121</v>
       </c>
-      <c r="G29" s="2" t="str">
-        <f aca="false">RIGHT(F29,3)</f>
-        <v>121</v>
+      <c r="G29" s="3" t="str">
+        <f aca="false">RIGHT(F29,2)</f>
+        <v>21</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="I29" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31121</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="n">
+      <c r="A30" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C30" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D30" s="2" t="str">
+      <c r="D30" s="4" t="str">
         <f aca="false">RIGHT(C30,2)</f>
         <v>11</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F30" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="F30" s="3" t="n">
         <v>311123</v>
       </c>
-      <c r="G30" s="2" t="str">
-        <f aca="false">RIGHT(F30,3)</f>
-        <v>123</v>
+      <c r="G30" s="3" t="str">
+        <f aca="false">RIGHT(F30,2)</f>
+        <v>23</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="I30" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31123</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="n">
+      <c r="A31" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C31" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D31" s="2" t="str">
+      <c r="D31" s="4" t="str">
         <f aca="false">RIGHT(C31,2)</f>
         <v>11</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F31" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="F31" s="3" t="n">
         <v>311124</v>
       </c>
-      <c r="G31" s="2" t="str">
-        <f aca="false">RIGHT(F31,3)</f>
-        <v>124</v>
+      <c r="G31" s="3" t="str">
+        <f aca="false">RIGHT(F31,2)</f>
+        <v>24</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="I31" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31124</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="n">
+      <c r="A32" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C32" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D32" s="2" t="str">
+      <c r="D32" s="4" t="str">
         <f aca="false">RIGHT(C32,2)</f>
         <v>11</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F32" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="F32" s="3" t="n">
         <v>311125</v>
       </c>
-      <c r="G32" s="2" t="str">
-        <f aca="false">RIGHT(F32,3)</f>
-        <v>125</v>
+      <c r="G32" s="3" t="str">
+        <f aca="false">RIGHT(F32,2)</f>
+        <v>25</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="I32" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31125</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="n">
+      <c r="A33" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C33" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D33" s="2" t="str">
+      <c r="D33" s="4" t="str">
         <f aca="false">RIGHT(C33,2)</f>
         <v>11</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F33" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="F33" s="3" t="n">
         <v>311127</v>
       </c>
-      <c r="G33" s="2" t="str">
-        <f aca="false">RIGHT(F33,3)</f>
-        <v>127</v>
+      <c r="G33" s="3" t="str">
+        <f aca="false">RIGHT(F33,2)</f>
+        <v>27</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="I33" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31127</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="n">
+      <c r="A34" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C34" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D34" s="2" t="str">
+      <c r="D34" s="4" t="str">
         <f aca="false">RIGHT(C34,2)</f>
         <v>11</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F34" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="F34" s="3" t="n">
         <v>311128</v>
       </c>
-      <c r="G34" s="2" t="str">
-        <f aca="false">RIGHT(F34,3)</f>
-        <v>128</v>
+      <c r="G34" s="3" t="str">
+        <f aca="false">RIGHT(F34,2)</f>
+        <v>28</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="I34" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31128</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="n">
+      <c r="A35" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C35" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D35" s="2" t="str">
+      <c r="D35" s="4" t="str">
         <f aca="false">RIGHT(C35,2)</f>
         <v>11</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F35" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="F35" s="3" t="n">
         <v>311129</v>
       </c>
-      <c r="G35" s="2" t="str">
-        <f aca="false">RIGHT(F35,3)</f>
-        <v>129</v>
+      <c r="G35" s="3" t="str">
+        <f aca="false">RIGHT(F35,2)</f>
+        <v>29</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="I35" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31129</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="n">
+      <c r="A36" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C36" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D36" s="2" t="str">
+      <c r="D36" s="4" t="str">
         <f aca="false">RIGHT(C36,2)</f>
         <v>11</v>
       </c>
       <c r="E36" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F36" s="3" t="n">
+        <v>311130</v>
+      </c>
+      <c r="G36" s="3" t="str">
+        <f aca="false">RIGHT(F36,2)</f>
         <v>30</v>
       </c>
-      <c r="F36" s="2" t="n">
-        <v>311130</v>
-      </c>
-      <c r="G36" s="2" t="str">
-        <f aca="false">RIGHT(F36,3)</f>
-        <v>130</v>
-      </c>
       <c r="H36" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="I36" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31130</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="n">
+      <c r="A37" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C37" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D37" s="2" t="str">
+      <c r="D37" s="4" t="str">
         <f aca="false">RIGHT(C37,2)</f>
         <v>11</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F37" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="F37" s="3" t="n">
         <v>311131</v>
       </c>
-      <c r="G37" s="2" t="str">
-        <f aca="false">RIGHT(F37,3)</f>
-        <v>131</v>
+      <c r="G37" s="3" t="str">
+        <f aca="false">RIGHT(F37,2)</f>
+        <v>31</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="I37" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31131</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2" t="n">
+      <c r="A38" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C38" s="3" t="n">
         <v>313</v>
       </c>
-      <c r="D38" s="2" t="str">
+      <c r="D38" s="4" t="str">
         <f aca="false">RIGHT(C38,2)</f>
         <v>13</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F38" s="2" t="n">
+        <v>52</v>
+      </c>
+      <c r="F38" s="3" t="n">
         <v>313301</v>
       </c>
-      <c r="G38" s="2" t="str">
-        <f aca="false">RIGHT(F38,3)</f>
-        <v>301</v>
+      <c r="G38" s="3" t="str">
+        <f aca="false">RIGHT(F38,2)</f>
+        <v>01</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="I38" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31301</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="n">
+      <c r="A39" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C39" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C39" s="3" t="n">
         <v>314</v>
       </c>
-      <c r="D39" s="2" t="str">
+      <c r="D39" s="4" t="str">
         <f aca="false">RIGHT(C39,2)</f>
         <v>14</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F39" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="F39" s="3" t="n">
         <v>314401</v>
       </c>
-      <c r="G39" s="2" t="str">
-        <f aca="false">RIGHT(F39,3)</f>
-        <v>401</v>
+      <c r="G39" s="3" t="str">
+        <f aca="false">RIGHT(F39,2)</f>
+        <v>01</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="I39" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31401</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="n">
+      <c r="A40" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C40" s="3" t="n">
         <v>314</v>
       </c>
-      <c r="D40" s="2" t="str">
+      <c r="D40" s="4" t="str">
         <f aca="false">RIGHT(C40,2)</f>
         <v>14</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F40" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="F40" s="3" t="n">
         <v>314402</v>
       </c>
-      <c r="G40" s="2" t="str">
-        <f aca="false">RIGHT(F40,3)</f>
-        <v>402</v>
+      <c r="G40" s="3" t="str">
+        <f aca="false">RIGHT(F40,2)</f>
+        <v>02</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="I40" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31402</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="n">
+      <c r="A41" s="3" t="n">
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C41" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="C41" s="3" t="n">
         <v>410</v>
       </c>
-      <c r="D41" s="2" t="str">
+      <c r="D41" s="4" t="str">
         <f aca="false">RIGHT(C41,2)</f>
         <v>10</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F41" s="3" t="n">
+        <v>410001</v>
+      </c>
+      <c r="G41" s="3" t="str">
+        <f aca="false">RIGHT(F41,2)</f>
+        <v>01</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I41" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>41001</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F41" s="2" t="n">
-        <v>410001</v>
-      </c>
-      <c r="G41" s="2" t="str">
-        <f aca="false">RIGHT(F41,3)</f>
-        <v>001</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C42" s="2" t="n">
+      <c r="C42" s="3" t="n">
         <v>410</v>
       </c>
-      <c r="D42" s="2" t="str">
+      <c r="D42" s="4" t="str">
         <f aca="false">RIGHT(C42,2)</f>
         <v>10</v>
       </c>
       <c r="E42" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F42" s="3" t="n">
+        <v>410002</v>
+      </c>
+      <c r="G42" s="3" t="str">
+        <f aca="false">RIGHT(F42,2)</f>
+        <v>02</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I42" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>41002</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F42" s="2" t="n">
-        <v>410002</v>
-      </c>
-      <c r="G42" s="2" t="str">
-        <f aca="false">RIGHT(F42,3)</f>
-        <v>002</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C43" s="2" t="n">
+      <c r="C43" s="3" t="n">
         <v>411</v>
       </c>
-      <c r="D43" s="2" t="str">
+      <c r="D43" s="4" t="str">
         <f aca="false">RIGHT(C43,2)</f>
         <v>11</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F43" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="F43" s="3" t="n">
         <v>411101</v>
       </c>
-      <c r="G43" s="2" t="str">
-        <f aca="false">RIGHT(F43,3)</f>
-        <v>101</v>
+      <c r="G43" s="3" t="str">
+        <f aca="false">RIGHT(F43,2)</f>
+        <v>01</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+      <c r="I43" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>41101</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="n">
+      <c r="A44" s="3" t="n">
         <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C44" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="C44" s="3" t="n">
         <v>411</v>
       </c>
-      <c r="D44" s="2" t="str">
+      <c r="D44" s="4" t="str">
         <f aca="false">RIGHT(C44,2)</f>
         <v>11</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F44" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="F44" s="3" t="n">
         <v>411102</v>
       </c>
-      <c r="G44" s="2" t="str">
-        <f aca="false">RIGHT(F44,3)</f>
-        <v>102</v>
+      <c r="G44" s="3" t="str">
+        <f aca="false">RIGHT(F44,2)</f>
+        <v>02</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="I44" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>41102</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="2" t="n">
+      <c r="A45" s="3" t="n">
         <v>4</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C45" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="C45" s="3" t="n">
         <v>411</v>
       </c>
-      <c r="D45" s="2" t="str">
+      <c r="D45" s="4" t="str">
         <f aca="false">RIGHT(C45,2)</f>
         <v>11</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F45" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="F45" s="3" t="n">
         <v>411104</v>
       </c>
-      <c r="G45" s="2" t="str">
-        <f aca="false">RIGHT(F45,3)</f>
-        <v>104</v>
+      <c r="G45" s="3" t="str">
+        <f aca="false">RIGHT(F45,2)</f>
+        <v>04</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
+      </c>
+      <c r="I45" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>41104</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="n">
+      <c r="A46" s="3" t="n">
         <v>4</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C46" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="C46" s="3" t="n">
         <v>412</v>
       </c>
-      <c r="D46" s="2" t="str">
+      <c r="D46" s="4" t="str">
         <f aca="false">RIGHT(C46,2)</f>
         <v>12</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F46" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="F46" s="3" t="n">
         <v>412201</v>
       </c>
-      <c r="G46" s="2" t="str">
-        <f aca="false">RIGHT(F46,3)</f>
-        <v>201</v>
+      <c r="G46" s="3" t="str">
+        <f aca="false">RIGHT(F46,2)</f>
+        <v>01</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="I46" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>41201</v>
       </c>
     </row>
     <row r="47" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2043,27 +2367,31 @@
         <v>5</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>510</v>
       </c>
-      <c r="D47" s="2" t="str">
+      <c r="D47" s="4" t="str">
         <f aca="false">RIGHT(C47,2)</f>
         <v>10</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F47" s="1" t="n">
         <v>510001</v>
       </c>
-      <c r="G47" s="2" t="str">
-        <f aca="false">RIGHT(F47,3)</f>
-        <v>001</v>
+      <c r="G47" s="3" t="str">
+        <f aca="false">RIGHT(F47,2)</f>
+        <v>01</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="I47" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>51001</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2071,111 +2399,127 @@
         <v>3</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C48" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C48" s="3" t="n">
         <v>312</v>
       </c>
-      <c r="D48" s="2" t="str">
+      <c r="D48" s="4" t="str">
         <f aca="false">RIGHT(C48,2)</f>
         <v>12</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F48" s="1" t="n">
         <v>311001</v>
       </c>
-      <c r="G48" s="2" t="str">
-        <f aca="false">RIGHT(F48,3)</f>
-        <v>001</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>66</v>
+      <c r="G48" s="3" t="str">
+        <f aca="false">RIGHT(F48,2)</f>
+        <v>01</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I48" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31201</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="2" t="n">
+      <c r="A49" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C49" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C49" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D49" s="2" t="str">
+      <c r="D49" s="4" t="str">
         <f aca="false">RIGHT(C49,2)</f>
         <v>11</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F49" s="1" t="n">
         <v>311116</v>
       </c>
-      <c r="G49" s="2" t="str">
-        <f aca="false">RIGHT(F49,3)</f>
-        <v>116</v>
+      <c r="G49" s="3" t="str">
+        <f aca="false">RIGHT(F49,2)</f>
+        <v>16</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="I49" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31116</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2" t="n">
+      <c r="A50" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C50" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C50" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D50" s="2" t="str">
+      <c r="D50" s="4" t="str">
         <f aca="false">RIGHT(C50,2)</f>
         <v>11</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F50" s="1" t="n">
         <v>311117</v>
       </c>
-      <c r="G50" s="2" t="str">
-        <f aca="false">RIGHT(F50,3)</f>
-        <v>117</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>68</v>
+      <c r="G50" s="3" t="str">
+        <f aca="false">RIGHT(F50,2)</f>
+        <v>17</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I50" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31117</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="2" t="n">
+      <c r="A51" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C51" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C51" s="3" t="n">
         <v>311</v>
       </c>
-      <c r="D51" s="2" t="str">
+      <c r="D51" s="4" t="str">
         <f aca="false">RIGHT(C51,2)</f>
         <v>11</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F51" s="1" t="n">
         <v>311118</v>
       </c>
-      <c r="G51" s="2" t="str">
-        <f aca="false">RIGHT(F51,3)</f>
-        <v>118</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>69</v>
+      <c r="G51" s="3" t="str">
+        <f aca="false">RIGHT(F51,2)</f>
+        <v>18</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I51" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31118</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2183,27 +2527,31 @@
         <v>3</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C52" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C52" s="3" t="n">
         <v>312</v>
       </c>
-      <c r="D52" s="2" t="str">
+      <c r="D52" s="4" t="str">
         <f aca="false">RIGHT(C52,2)</f>
         <v>12</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F52" s="1" t="n">
         <v>311002</v>
       </c>
-      <c r="G52" s="2" t="str">
-        <f aca="false">RIGHT(F52,3)</f>
-        <v>002</v>
+      <c r="G52" s="3" t="str">
+        <f aca="false">RIGHT(F52,2)</f>
+        <v>02</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="I52" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31202</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2211,27 +2559,521 @@
         <v>3</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C53" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C53" s="3" t="n">
         <v>312</v>
       </c>
-      <c r="D53" s="2" t="str">
+      <c r="D53" s="4" t="str">
         <f aca="false">RIGHT(C53,2)</f>
         <v>12</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F53" s="1" t="n">
         <v>311003</v>
       </c>
-      <c r="G53" s="2" t="str">
-        <f aca="false">RIGHT(F53,3)</f>
-        <v>003</v>
+      <c r="G53" s="3" t="str">
+        <f aca="false">RIGHT(F53,2)</f>
+        <v>03</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="I53" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31203</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" s="3" t="n">
+        <v>312</v>
+      </c>
+      <c r="D54" s="4" t="str">
+        <f aca="false">RIGHT(C54,2)</f>
+        <v>12</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F54" s="1" t="n">
+        <v>311004</v>
+      </c>
+      <c r="G54" s="3" t="str">
+        <f aca="false">RIGHT(F54,2)</f>
+        <v>04</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I54" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31204</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="D55" s="4" t="str">
+        <f aca="false">RIGHT(C55,2)</f>
+        <v>19</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F55" s="1" t="n">
+        <v>119001</v>
+      </c>
+      <c r="G55" s="3" t="str">
+        <f aca="false">RIGHT(F55,2)</f>
+        <v>01</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I55" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>11901</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C56" s="3" t="n">
+        <v>311</v>
+      </c>
+      <c r="D56" s="4" t="str">
+        <f aca="false">RIGHT(C56,2)</f>
+        <v>11</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F56" s="1" t="n">
+        <v>311119</v>
+      </c>
+      <c r="G56" s="3" t="str">
+        <f aca="false">RIGHT(F56,2)</f>
+        <v>19</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I56" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>31119</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C57" s="1" t="n">
+        <v>803</v>
+      </c>
+      <c r="D57" s="4" t="str">
+        <f aca="false">RIGHT(C57,2)</f>
+        <v>03</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F57" s="1" t="n">
+        <v>803003</v>
+      </c>
+      <c r="G57" s="3" t="str">
+        <f aca="false">RIGHT(F57,2)</f>
+        <v>03</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I57" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>80303</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C58" s="1" t="n">
+        <v>804</v>
+      </c>
+      <c r="D58" s="4" t="str">
+        <f aca="false">RIGHT(C58,2)</f>
+        <v>04</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F58" s="1" t="n">
+        <v>804003</v>
+      </c>
+      <c r="G58" s="3" t="str">
+        <f aca="false">RIGHT(F58,2)</f>
+        <v>03</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I58" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>80403</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="D59" s="4" t="str">
+        <f aca="false">RIGHT(C59,2)</f>
+        <v>20</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F59" s="1" t="n">
+        <v>120001</v>
+      </c>
+      <c r="G59" s="3" t="str">
+        <f aca="false">RIGHT(F59,2)</f>
+        <v>01</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I59" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>12001</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="D60" s="4" t="str">
+        <f aca="false">RIGHT(C60,2)</f>
+        <v>20</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F60" s="1" t="n">
+        <v>120002</v>
+      </c>
+      <c r="G60" s="3" t="str">
+        <f aca="false">RIGHT(F60,2)</f>
+        <v>02</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I60" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>12002</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="D61" s="4" t="str">
+        <f aca="false">RIGHT(C61,2)</f>
+        <v>20</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F61" s="1" t="n">
+        <v>120003</v>
+      </c>
+      <c r="G61" s="3" t="str">
+        <f aca="false">RIGHT(F61,2)</f>
+        <v>03</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I61" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>12003</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="D62" s="4" t="str">
+        <f aca="false">RIGHT(C62,2)</f>
+        <v>20</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F62" s="1" t="n">
+        <v>120004</v>
+      </c>
+      <c r="G62" s="3" t="str">
+        <f aca="false">RIGHT(F62,2)</f>
+        <v>04</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I62" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>12004</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="D63" s="4" t="str">
+        <f aca="false">RIGHT(C63,2)</f>
+        <v>20</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F63" s="1" t="n">
+        <v>120005</v>
+      </c>
+      <c r="G63" s="3" t="str">
+        <f aca="false">RIGHT(F63,2)</f>
+        <v>05</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I63" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(new[[#This Row],[cat_id]],new[[#This Row],[segment_id]],new[[#This Row],[m_segment_id]])</f>
+        <v>12005</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="D64" s="4" t="str">
+        <f aca="false">RIGHT(C64,2)</f>
+        <v>20</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F64" s="1" t="n">
+        <v>120006</v>
+      </c>
+      <c r="G64" s="3" t="str">
+        <f aca="false">RIGHT(F64,2)</f>
+        <v>06</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I64" s="1" t="n">
+        <v>12006</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C65" s="1" t="n">
+        <v>801</v>
+      </c>
+      <c r="D65" s="4" t="str">
+        <f aca="false">RIGHT(C65,2)</f>
+        <v>01</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I65" s="1" t="n">
+        <v>80104</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C66" s="1" t="n">
+        <v>802</v>
+      </c>
+      <c r="D66" s="4" t="str">
+        <f aca="false">RIGHT(C66,2)</f>
+        <v>02</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I66" s="1" t="n">
+        <v>80204</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="D67" s="4" t="str">
+        <f aca="false">RIGHT(C67,2)</f>
+        <v>20</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F67" s="1" t="n">
+        <v>120007</v>
+      </c>
+      <c r="G67" s="3" t="str">
+        <f aca="false">RIGHT(F67,2)</f>
+        <v>07</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I67" s="1" t="n">
+        <v>12007</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C68" s="3" t="n">
+        <v>311</v>
+      </c>
+      <c r="D68" s="4" t="str">
+        <f aca="false">RIGHT(C68,2)</f>
+        <v>11</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G68" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I68" s="1" t="n">
+        <v>31132</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" s="3" t="n">
+        <v>118</v>
+      </c>
+      <c r="D69" s="4" t="str">
+        <f aca="false">RIGHT(C69,2)</f>
+        <v>18</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G69" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I69" s="1" t="n">
+        <v>11810</v>
       </c>
     </row>
   </sheetData>

</xml_diff>